<commit_message>
modify and check spcotmhp codes
</commit_message>
<xml_diff>
--- a/SIGVerse/dataset/similar/3LDK/3LDK_05/position/3LDK_5_position.xlsx
+++ b/SIGVerse/dataset/similar/3LDK/3LDK_05/position/3LDK_5_position.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="3LDK_5_position" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -50,13 +50,6 @@
     <phoneticPr fontId="18"/>
   </si>
   <si>
-    <t>廊下</t>
-    <rPh sb="0" eb="2">
-      <t>ロウカ</t>
-    </rPh>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
     <t>きいろ</t>
     <phoneticPr fontId="18"/>
   </si>
@@ -80,6 +73,16 @@
   </si>
   <si>
     <t>みどり</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>玄関 廊下</t>
+    <rPh sb="0" eb="2">
+      <t>ゲンカン</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ロウカ</t>
+    </rPh>
     <phoneticPr fontId="18"/>
   </si>
 </sst>
@@ -673,8 +676,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -824,54 +830,54 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'3LDK_5_position'!$C$2:$C$151</c:f>
+              <c:f>'3LDK_5_position'!$C$2:$C$166</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="150"/>
+                <c:ptCount val="165"/>
                 <c:pt idx="0">
-                  <c:v>5.52</c:v>
+                  <c:v>-0.55199999999999994</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>5.98</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.17</c:v>
+                  <c:v>5.5529999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.37</c:v>
+                  <c:v>1.274</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.57</c:v>
+                  <c:v>1.9710000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.65</c:v>
+                  <c:v>2.66</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>6.57</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.15</c:v>
+                  <c:v>3.69</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.22</c:v>
+                  <c:v>4.3539999999999992</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.92</c:v>
+                  <c:v>4.7359999999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.57</c:v>
+                  <c:v>0.55700000000000005</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>5.71</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.96</c:v>
+                  <c:v>0.96</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5.9</c:v>
+                  <c:v>2.95</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6.4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>6.61</c:v>
@@ -1277,16 +1283,61 @@
                 </c:pt>
                 <c:pt idx="149">
                   <c:v>4.2300000000000004</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>-1.6799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>-1.6900000000000004</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>-1.79</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>-1.9400000000000004</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>-2.38</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>-2.7300000000000004</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>-2.99</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>-3.2199999999999998</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>-3.1799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>-3.2199999999999998</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>-3.3099999999999996</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>-3.13</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>-2.8099999999999996</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>-2.5099999999999998</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>-2.3099999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'3LDK_5_position'!$D$2:$D$151</c:f>
+              <c:f>'3LDK_5_position'!$D$2:$D$166</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="150"/>
+                <c:ptCount val="165"/>
                 <c:pt idx="0">
                   <c:v>-0.43</c:v>
                 </c:pt>
@@ -1736,6 +1787,51 @@
                 </c:pt>
                 <c:pt idx="149">
                   <c:v>0.23</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>-1.03</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>-0.61</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>-0.05</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>0.27</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>-0.38</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>-0.82</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>-1.28</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>-1.1599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>-1.35</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>-1.27</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>-1.44</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2655,7 +2751,10 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="l"/>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>　　</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -3739,15 +3838,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R151"/>
+  <dimension ref="A1:Z166"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R31" sqref="R31"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3766,8 +3865,18 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="X1">
+        <v>5.52</v>
+      </c>
+      <c r="Y1">
+        <v>-0.1</v>
+      </c>
+      <c r="Z1">
+        <f>X1*Y1</f>
+        <v>-0.55199999999999994</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>0</v>
       </c>
@@ -3775,7 +3884,7 @@
         <v>157.06</v>
       </c>
       <c r="C2">
-        <v>5.52</v>
+        <v>-0.55199999999999994</v>
       </c>
       <c r="D2">
         <v>-0.43</v>
@@ -3786,8 +3895,18 @@
       <c r="F2">
         <v>0.92091352130000004</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="X2">
+        <v>5.98</v>
+      </c>
+      <c r="Y2">
+        <v>1</v>
+      </c>
+      <c r="Z2">
+        <f t="shared" ref="Z2:Z15" si="0">X2*Y2</f>
+        <v>5.98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3806,8 +3925,18 @@
       <c r="F3">
         <v>0.99706612699999997</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="X3">
+        <v>6.17</v>
+      </c>
+      <c r="Y3">
+        <v>0.9</v>
+      </c>
+      <c r="Z3">
+        <f t="shared" si="0"/>
+        <v>5.5529999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>2</v>
       </c>
@@ -3815,7 +3944,7 @@
         <v>146.34</v>
       </c>
       <c r="C4">
-        <v>6.17</v>
+        <v>5.5529999999999999</v>
       </c>
       <c r="D4">
         <v>-0.45</v>
@@ -3826,8 +3955,18 @@
       <c r="F4">
         <v>0.8323412738</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="X4">
+        <v>6.37</v>
+      </c>
+      <c r="Y4">
+        <v>0.2</v>
+      </c>
+      <c r="Z4">
+        <f t="shared" si="0"/>
+        <v>1.274</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>3</v>
       </c>
@@ -3835,7 +3974,7 @@
         <v>153.44</v>
       </c>
       <c r="C5">
-        <v>6.37</v>
+        <v>1.274</v>
       </c>
       <c r="D5">
         <v>-0.49</v>
@@ -3846,8 +3985,18 @@
       <c r="F5">
         <v>0.89446661370000002</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="X5">
+        <v>6.57</v>
+      </c>
+      <c r="Y5">
+        <v>0.3</v>
+      </c>
+      <c r="Z5">
+        <f t="shared" si="0"/>
+        <v>1.9710000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>4</v>
       </c>
@@ -3855,7 +4004,7 @@
         <v>80.95</v>
       </c>
       <c r="C6">
-        <v>6.57</v>
+        <v>1.9710000000000001</v>
       </c>
       <c r="D6">
         <v>-0.46</v>
@@ -3866,8 +4015,18 @@
       <c r="F6">
         <v>-0.15729632599999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="X6">
+        <v>6.65</v>
+      </c>
+      <c r="Y6">
+        <v>0.4</v>
+      </c>
+      <c r="Z6">
+        <f t="shared" si="0"/>
+        <v>2.66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>5</v>
       </c>
@@ -3875,7 +4034,7 @@
         <v>83.33</v>
       </c>
       <c r="C7">
-        <v>6.65</v>
+        <v>2.66</v>
       </c>
       <c r="D7">
         <v>-0.82</v>
@@ -3886,8 +4045,18 @@
       <c r="F7">
         <v>-0.1161506982</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="X7">
+        <v>6.57</v>
+      </c>
+      <c r="Y7">
+        <v>1</v>
+      </c>
+      <c r="Z7">
+        <f t="shared" si="0"/>
+        <v>6.57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>6</v>
       </c>
@@ -3906,8 +4075,18 @@
       <c r="F8">
         <v>-0.1493627706</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="X8">
+        <v>6.15</v>
+      </c>
+      <c r="Y8">
+        <v>0.6</v>
+      </c>
+      <c r="Z8">
+        <f t="shared" si="0"/>
+        <v>3.69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>7</v>
       </c>
@@ -3915,7 +4094,7 @@
         <v>177.6</v>
       </c>
       <c r="C9">
-        <v>6.15</v>
+        <v>3.69</v>
       </c>
       <c r="D9">
         <v>-1.07</v>
@@ -3926,8 +4105,18 @@
       <c r="F9">
         <v>0.99912283010000003</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="X9">
+        <v>6.22</v>
+      </c>
+      <c r="Y9">
+        <v>0.7</v>
+      </c>
+      <c r="Z9">
+        <f t="shared" si="0"/>
+        <v>4.3539999999999992</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>8</v>
       </c>
@@ -3935,7 +4124,7 @@
         <v>172.73</v>
       </c>
       <c r="C10">
-        <v>6.22</v>
+        <v>4.3539999999999992</v>
       </c>
       <c r="D10">
         <v>-0.82</v>
@@ -3946,8 +4135,18 @@
       <c r="F10">
         <v>0.99196083749999997</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="X10">
+        <v>5.92</v>
+      </c>
+      <c r="Y10">
+        <v>0.8</v>
+      </c>
+      <c r="Z10">
+        <f t="shared" si="0"/>
+        <v>4.7359999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>9</v>
       </c>
@@ -3955,7 +4154,7 @@
         <v>168.98</v>
       </c>
       <c r="C11">
-        <v>5.92</v>
+        <v>4.7359999999999998</v>
       </c>
       <c r="D11">
         <v>-0.8</v>
@@ -3966,8 +4165,18 @@
       <c r="F11">
         <v>0.98156051870000005</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="X11">
+        <v>5.57</v>
+      </c>
+      <c r="Y11">
+        <v>0.1</v>
+      </c>
+      <c r="Z11">
+        <f t="shared" si="0"/>
+        <v>0.55700000000000005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>10</v>
       </c>
@@ -3975,7 +4184,7 @@
         <v>176.39</v>
       </c>
       <c r="C12">
-        <v>5.57</v>
+        <v>0.55700000000000005</v>
       </c>
       <c r="D12">
         <v>-0.82</v>
@@ -3986,8 +4195,18 @@
       <c r="F12">
         <v>0.99801575419999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="X12">
+        <v>5.71</v>
+      </c>
+      <c r="Y12">
+        <v>1</v>
+      </c>
+      <c r="Z12">
+        <f t="shared" si="0"/>
+        <v>5.71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>11</v>
       </c>
@@ -4006,8 +4225,18 @@
       <c r="F13">
         <v>0.60083885690000005</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="X13">
+        <v>5.96</v>
+      </c>
+      <c r="Y13">
+        <v>1</v>
+      </c>
+      <c r="Z13">
+        <f t="shared" si="0"/>
+        <v>5.96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>12</v>
       </c>
@@ -4015,7 +4244,7 @@
         <v>-164.28</v>
       </c>
       <c r="C14">
-        <v>5.96</v>
+        <v>0.96</v>
       </c>
       <c r="D14">
         <v>-1.8</v>
@@ -4026,8 +4255,18 @@
       <c r="F14">
         <v>0.9625972304</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="X14">
+        <v>5.9</v>
+      </c>
+      <c r="Y14">
+        <v>0.5</v>
+      </c>
+      <c r="Z14">
+        <f t="shared" si="0"/>
+        <v>2.95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>13</v>
       </c>
@@ -4035,7 +4274,7 @@
         <v>-172.83</v>
       </c>
       <c r="C15">
-        <v>5.9</v>
+        <v>2.95</v>
       </c>
       <c r="D15">
         <v>-1.43</v>
@@ -4046,8 +4285,18 @@
       <c r="F15">
         <v>0.99218018959999998</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="X15">
+        <v>6.4</v>
+      </c>
+      <c r="Y15">
+        <v>0</v>
+      </c>
+      <c r="Z15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>14</v>
       </c>
@@ -4055,7 +4304,7 @@
         <v>-172.8</v>
       </c>
       <c r="C16">
-        <v>6.4</v>
+        <v>0</v>
       </c>
       <c r="D16">
         <v>-1.49</v>
@@ -4273,7 +4522,7 @@
         <v>7</v>
       </c>
       <c r="R26" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.15">
@@ -4296,7 +4545,7 @@
         <v>3.5771616300000003E-2</v>
       </c>
       <c r="R27" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.15">
@@ -4339,13 +4588,13 @@
         <v>-3.6818123899999999E-2</v>
       </c>
       <c r="P29" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q29" t="s">
         <v>10</v>
       </c>
-      <c r="Q29" t="s">
+      <c r="R29" t="s">
         <v>11</v>
-      </c>
-      <c r="R29" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.15">
@@ -4368,7 +4617,7 @@
         <v>0.2038126237</v>
       </c>
       <c r="R30" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.15">
@@ -6651,7 +6900,7 @@
         <v>0.88741344710000003</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A145">
         <v>143</v>
       </c>
@@ -6671,7 +6920,7 @@
         <v>0.86349239700000002</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A146">
         <v>144</v>
       </c>
@@ -6691,7 +6940,7 @@
         <v>0.65803260350000004</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A147">
         <v>145</v>
       </c>
@@ -6711,7 +6960,7 @@
         <v>0.41135528249999997</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A148">
         <v>146</v>
       </c>
@@ -6731,7 +6980,7 @@
         <v>0.29887424130000001</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A149">
         <v>147</v>
       </c>
@@ -6751,7 +7000,7 @@
         <v>0.61648634049999995</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A150">
         <v>148</v>
       </c>
@@ -6771,7 +7020,7 @@
         <v>0.80468660609999998</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A151">
         <v>149</v>
       </c>
@@ -6789,11 +7038,399 @@
       </c>
       <c r="F151">
         <v>0.92274002290000001</v>
+      </c>
+    </row>
+    <row r="152" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A152" s="1">
+        <v>150</v>
+      </c>
+      <c r="C152">
+        <v>-1.6799999999999997</v>
+      </c>
+      <c r="D152">
+        <v>-1.03</v>
+      </c>
+      <c r="H152">
+        <v>-4.68</v>
+      </c>
+      <c r="I152">
+        <v>-1.03</v>
+      </c>
+      <c r="J152">
+        <v>3</v>
+      </c>
+      <c r="K152">
+        <f>H152+J152</f>
+        <v>-1.6799999999999997</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A153" s="1">
+        <v>151</v>
+      </c>
+      <c r="C153">
+        <v>-1.6900000000000004</v>
+      </c>
+      <c r="D153">
+        <v>-0.61</v>
+      </c>
+      <c r="H153">
+        <v>-4.6900000000000004</v>
+      </c>
+      <c r="I153">
+        <v>-0.61</v>
+      </c>
+      <c r="J153">
+        <v>3</v>
+      </c>
+      <c r="K153">
+        <f t="shared" ref="K153:K166" si="1">H153+J153</f>
+        <v>-1.6900000000000004</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A154" s="1">
+        <v>152</v>
+      </c>
+      <c r="C154">
+        <v>-1.79</v>
+      </c>
+      <c r="D154">
+        <v>-0.05</v>
+      </c>
+      <c r="H154">
+        <v>-4.79</v>
+      </c>
+      <c r="I154">
+        <v>-0.05</v>
+      </c>
+      <c r="J154">
+        <v>3</v>
+      </c>
+      <c r="K154">
+        <f t="shared" si="1"/>
+        <v>-1.79</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A155" s="1">
+        <v>153</v>
+      </c>
+      <c r="C155">
+        <v>-1.9400000000000004</v>
+      </c>
+      <c r="D155">
+        <v>0.35</v>
+      </c>
+      <c r="H155">
+        <v>-4.9400000000000004</v>
+      </c>
+      <c r="I155">
+        <v>0.35</v>
+      </c>
+      <c r="J155">
+        <v>3</v>
+      </c>
+      <c r="K155">
+        <f t="shared" si="1"/>
+        <v>-1.9400000000000004</v>
+      </c>
+    </row>
+    <row r="156" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A156" s="1">
+        <v>154</v>
+      </c>
+      <c r="C156">
+        <v>-2.38</v>
+      </c>
+      <c r="D156">
+        <v>0.22</v>
+      </c>
+      <c r="H156">
+        <v>-5.38</v>
+      </c>
+      <c r="I156">
+        <v>0.22</v>
+      </c>
+      <c r="J156">
+        <v>3</v>
+      </c>
+      <c r="K156">
+        <f t="shared" si="1"/>
+        <v>-2.38</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A157" s="1">
+        <v>155</v>
+      </c>
+      <c r="C157">
+        <v>-2.7300000000000004</v>
+      </c>
+      <c r="D157">
+        <v>0.27</v>
+      </c>
+      <c r="H157">
+        <v>-5.73</v>
+      </c>
+      <c r="I157">
+        <v>0.27</v>
+      </c>
+      <c r="J157">
+        <v>3</v>
+      </c>
+      <c r="K157">
+        <f t="shared" si="1"/>
+        <v>-2.7300000000000004</v>
+      </c>
+    </row>
+    <row r="158" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A158" s="1">
+        <v>156</v>
+      </c>
+      <c r="C158">
+        <v>-2.99</v>
+      </c>
+      <c r="D158">
+        <v>0.24</v>
+      </c>
+      <c r="H158">
+        <v>-5.99</v>
+      </c>
+      <c r="I158">
+        <v>0.24</v>
+      </c>
+      <c r="J158">
+        <v>3</v>
+      </c>
+      <c r="K158">
+        <f t="shared" si="1"/>
+        <v>-2.99</v>
+      </c>
+    </row>
+    <row r="159" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A159" s="1">
+        <v>157</v>
+      </c>
+      <c r="C159">
+        <v>-3.2199999999999998</v>
+      </c>
+      <c r="D159">
+        <v>0.1</v>
+      </c>
+      <c r="H159">
+        <v>-6.22</v>
+      </c>
+      <c r="I159">
+        <v>0.1</v>
+      </c>
+      <c r="J159">
+        <v>3</v>
+      </c>
+      <c r="K159">
+        <f t="shared" si="1"/>
+        <v>-3.2199999999999998</v>
+      </c>
+    </row>
+    <row r="160" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A160" s="1">
+        <v>158</v>
+      </c>
+      <c r="C160">
+        <v>-3.1799999999999997</v>
+      </c>
+      <c r="D160">
+        <v>-0.38</v>
+      </c>
+      <c r="H160">
+        <v>-6.18</v>
+      </c>
+      <c r="I160">
+        <v>-0.38</v>
+      </c>
+      <c r="J160">
+        <v>3</v>
+      </c>
+      <c r="K160">
+        <f t="shared" si="1"/>
+        <v>-3.1799999999999997</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A161" s="1">
+        <v>159</v>
+      </c>
+      <c r="C161">
+        <v>-3.2199999999999998</v>
+      </c>
+      <c r="D161">
+        <v>-0.82</v>
+      </c>
+      <c r="H161">
+        <v>-6.22</v>
+      </c>
+      <c r="I161">
+        <v>-0.82</v>
+      </c>
+      <c r="J161">
+        <v>3</v>
+      </c>
+      <c r="K161">
+        <f t="shared" si="1"/>
+        <v>-3.2199999999999998</v>
+      </c>
+    </row>
+    <row r="162" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A162" s="1">
+        <v>160</v>
+      </c>
+      <c r="C162">
+        <v>-3.3099999999999996</v>
+      </c>
+      <c r="D162">
+        <v>-1.28</v>
+      </c>
+      <c r="H162">
+        <v>-6.31</v>
+      </c>
+      <c r="I162">
+        <v>-1.28</v>
+      </c>
+      <c r="J162">
+        <v>3</v>
+      </c>
+      <c r="K162">
+        <f t="shared" si="1"/>
+        <v>-3.3099999999999996</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A163" s="1">
+        <v>161</v>
+      </c>
+      <c r="C163">
+        <v>-3.13</v>
+      </c>
+      <c r="D163">
+        <v>-1.1599999999999999</v>
+      </c>
+      <c r="H163">
+        <v>-6.13</v>
+      </c>
+      <c r="I163">
+        <v>-1.1599999999999999</v>
+      </c>
+      <c r="J163">
+        <v>3</v>
+      </c>
+      <c r="K163">
+        <f t="shared" si="1"/>
+        <v>-3.13</v>
+      </c>
+    </row>
+    <row r="164" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A164" s="1">
+        <v>162</v>
+      </c>
+      <c r="C164">
+        <v>-2.8099999999999996</v>
+      </c>
+      <c r="D164">
+        <v>-1.35</v>
+      </c>
+      <c r="H164">
+        <v>-5.81</v>
+      </c>
+      <c r="I164">
+        <v>-1.35</v>
+      </c>
+      <c r="J164">
+        <v>3</v>
+      </c>
+      <c r="K164">
+        <f t="shared" si="1"/>
+        <v>-2.8099999999999996</v>
+      </c>
+    </row>
+    <row r="165" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A165" s="1">
+        <v>163</v>
+      </c>
+      <c r="C165">
+        <v>-2.5099999999999998</v>
+      </c>
+      <c r="D165">
+        <v>-1.27</v>
+      </c>
+      <c r="H165">
+        <v>-5.51</v>
+      </c>
+      <c r="I165">
+        <v>-1.27</v>
+      </c>
+      <c r="J165">
+        <v>3</v>
+      </c>
+      <c r="K165">
+        <f t="shared" si="1"/>
+        <v>-2.5099999999999998</v>
+      </c>
+    </row>
+    <row r="166" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="A166" s="1">
+        <v>164</v>
+      </c>
+      <c r="C166">
+        <v>-2.3099999999999996</v>
+      </c>
+      <c r="D166">
+        <v>-1.44</v>
+      </c>
+      <c r="H166">
+        <v>-5.31</v>
+      </c>
+      <c r="I166">
+        <v>-1.44</v>
+      </c>
+      <c r="J166">
+        <v>3</v>
+      </c>
+      <c r="K166">
+        <f t="shared" si="1"/>
+        <v>-2.3099999999999996</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18"/>
   <conditionalFormatting sqref="C1:D1048576">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{E55CFA17-D032-4FD8-8F99-16D2B0D543F0}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X1:X15">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{BDD3A634-6811-4A96-980D-48A0698DF5FB}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H152:I166">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="min"/>
@@ -6802,7 +7439,7 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{E55CFA17-D032-4FD8-8F99-16D2B0D543F0}</x14:id>
+          <x14:id>{BED90FF9-A53E-4240-969F-A46E8D2D4D7A}</x14:id>
         </ext>
       </extLst>
     </cfRule>
@@ -6826,6 +7463,32 @@
           </x14:cfRule>
           <xm:sqref>C1:D1048576</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{BDD3A634-6811-4A96-980D-48A0698DF5FB}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>X1:X15</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{BED90FF9-A53E-4240-969F-A46E8D2D4D7A}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF638EC6"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H152:I166</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>

</xml_diff>